<commit_message>
ligegyldig ændring i test-xlxs-filen
</commit_message>
<xml_diff>
--- a/sample_employee_data.xlsx
+++ b/sample_employee_data.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luqma\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8AAEE6F-FC11-42A5-AD87-8EC68298714B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -74,13 +80,16 @@
   </si>
   <si>
     <t>2023-05-08</t>
+  </si>
+  <si>
+    <t>Tester</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,24 +141,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -187,7 +205,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -221,6 +239,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -255,9 +274,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -430,14 +450,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,8 +478,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -470,8 +498,11 @@
       <c r="E2" t="s">
         <v>15</v>
       </c>
+      <c r="F2">
+        <v>4000</v>
+      </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -487,8 +518,11 @@
       <c r="E3" t="s">
         <v>16</v>
       </c>
+      <c r="F3">
+        <v>3000</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -504,8 +538,11 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
+      <c r="F4">
+        <v>2000</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -521,8 +558,11 @@
       <c r="E5" t="s">
         <v>18</v>
       </c>
+      <c r="F5">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -537,6 +577,9 @@
       </c>
       <c r="E6" t="s">
         <v>19</v>
+      </c>
+      <c r="F6">
+        <v>600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>